<commit_message>
Add method to get data from an excel file.
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walis\OneDrive\Saga\Arquivos\Projetos\JAVA\whatsappbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walis\OneDrive\Saga\Arquivos\GitHub\whatsappbot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90C9BF0-5913-4BF2-A6B5-3F7B32591348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F749F9EE-B2DC-49DB-9715-21107D4825CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="1635" windowWidth="14520" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8670" yWindow="1185" windowWidth="20130" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,16 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>This is a test.</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,8 +59,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,23 +343,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="A1:E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" t="s" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="s" s="0">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Send messages and await until they're send.
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walis\OneDrive\Saga\Arquivos\GitHub\whatsappbot\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F749F9EE-B2DC-49DB-9715-21107D4825CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51DB9C7-5B89-4341-A7C6-CB9DE5C0E58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8670" yWindow="1185" windowWidth="20130" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8190" yWindow="1485" windowWidth="20085" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Message Status</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -59,10 +77,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,20 +364,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>